<commit_message>
Filter on errors in data, function to plot data
</commit_message>
<xml_diff>
--- a/To Do.xlsx
+++ b/To Do.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="31">
   <si>
     <t>Experiment GUI</t>
   </si>
@@ -91,6 +91,24 @@
   </si>
   <si>
     <t>Experiment</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Meh</t>
+  </si>
+  <si>
+    <t>Graph y axis closer to values</t>
+  </si>
+  <si>
+    <t>Filter data - remove garbage values</t>
+  </si>
+  <si>
+    <t>Notes in excel</t>
+  </si>
+  <si>
+    <t>Function stuff out</t>
   </si>
 </sst>
 </file>
@@ -458,10 +476,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B29"/>
+  <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -470,124 +488,174 @@
     <col min="2" max="2" width="51" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
       <c r="B2" s="2"/>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>24</v>
       </c>
       <c r="B9" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
+      <c r="C13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="C14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>15</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B18" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
+      <c r="C18" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>14</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B22" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="1" t="s">
+      <c r="C23" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
+    <row r="28" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
         <v>7</v>
+      </c>
+      <c r="C32" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Date stamp added to data and file name
</commit_message>
<xml_diff>
--- a/To Do.xlsx
+++ b/To Do.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="31">
   <si>
     <t>Experiment GUI</t>
   </si>
@@ -179,7 +179,22 @@
     <cellStyle name="Heading 2" xfId="1" builtinId="17"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -476,10 +491,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C32"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -524,18 +539,32 @@
       <c r="B6" t="s">
         <v>13</v>
       </c>
+      <c r="C6" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>10</v>
       </c>
+      <c r="C7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>24</v>
-      </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C9" t="s">
         <v>25</v>
@@ -543,33 +572,33 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>22</v>
+        <v>21</v>
+      </c>
+      <c r="C12" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="C13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="C14" t="s">
         <v>25</v>
@@ -577,89 +606,96 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>30</v>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>15</v>
-      </c>
       <c r="B18" t="s">
-        <v>16</v>
-      </c>
-      <c r="C18" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>14</v>
+      </c>
       <c r="B19" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>14</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="C20" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>8</v>
-      </c>
-      <c r="C23" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
+      <c r="C25" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
         <v>7</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C26" t="s">
         <v>26</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="C3:C20 C22:C26">
+    <cfRule type="containsBlanks" dxfId="1" priority="1">
+      <formula>LEN(TRIM(C3))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Basically all done, showed to Richard
</commit_message>
<xml_diff>
--- a/To Do.xlsx
+++ b/To Do.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="31">
   <si>
     <t>Experiment GUI</t>
   </si>
@@ -179,14 +179,7 @@
     <cellStyle name="Heading 2" xfId="1" builtinId="17"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <fill>
         <patternFill>
@@ -494,7 +487,7 @@
   <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -534,6 +527,9 @@
       <c r="B5" t="s">
         <v>12</v>
       </c>
+      <c r="C5" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
@@ -579,6 +575,9 @@
       <c r="B11" t="s">
         <v>22</v>
       </c>
+      <c r="C11" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
@@ -632,6 +631,9 @@
       <c r="B18" t="s">
         <v>29</v>
       </c>
+      <c r="C18" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
@@ -690,7 +692,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C3:C20 C22:C26">
-    <cfRule type="containsBlanks" dxfId="1" priority="1">
+    <cfRule type="containsBlanks" dxfId="0" priority="1">
       <formula>LEN(TRIM(C3))=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Tidied and fixed y-axis scale
</commit_message>
<xml_diff>
--- a/To Do.xlsx
+++ b/To Do.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="31">
   <si>
     <t>Experiment GUI</t>
   </si>
@@ -487,7 +487,7 @@
   <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -570,6 +570,9 @@
       <c r="B10" t="s">
         <v>27</v>
       </c>
+      <c r="C10" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
@@ -606,6 +609,9 @@
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>30</v>
+      </c>
+      <c r="C15" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Working code, Katelyn out
</commit_message>
<xml_diff>
--- a/To Do.xlsx
+++ b/To Do.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="36">
   <si>
     <t>Experiment GUI</t>
   </si>
@@ -109,6 +109,21 @@
   </si>
   <si>
     <t>Function stuff out</t>
+  </si>
+  <si>
+    <t>Dewpoint gives error with 0 humidity (likely a divide by zero issue)</t>
+  </si>
+  <si>
+    <t>Current data likely needs to be two separate dictionaries: when an error occurs, one sensor is pulling data from currentdata and that could actually be the data of the other sensor</t>
+  </si>
+  <si>
+    <t>Check in arduino that it isn't sending 255 from a sensor: make anything over 255 into 254</t>
+  </si>
+  <si>
+    <t>X axis… put time in here</t>
+  </si>
+  <si>
+    <t>Katelyn Gone Now</t>
   </si>
 </sst>
 </file>
@@ -484,10 +499,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -694,6 +709,31 @@
       </c>
       <c r="C26" t="s">
         <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>